<commit_message>
Atualização do andamento do Site Institucional
</commit_message>
<xml_diff>
--- a/Tecnologia da Informação/Backlog.xlsx
+++ b/Tecnologia da Informação/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/giulia_ayres_sptech_school/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/giulia_ayres_sptech_school/Documents/Giulia/Projeto-Diwine/Tecnologia da Informação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="943" documentId="8_{F8D6D5E0-FEAD-4D71-95E1-08BB12FF2741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF4E977B-57F1-455A-A7B6-13AE94C0D1A5}"/>
+  <xr:revisionPtr revIDLastSave="1094" documentId="8_{F8D6D5E0-FEAD-4D71-95E1-08BB12FF2741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6E5F817-3A79-405F-91DF-F6B7D1E239B8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="1" xr2:uid="{9BAA43A6-2120-409E-B19A-63F3A8B8DC14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9BAA43A6-2120-409E-B19A-63F3A8B8DC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="61">
   <si>
     <t>REQUISITO</t>
   </si>
@@ -73,6 +73,9 @@
     <t>Funcional</t>
   </si>
   <si>
+    <t>PP</t>
+  </si>
+  <si>
     <t>SP3</t>
   </si>
   <si>
@@ -96,6 +99,9 @@
     <t>O login deverá ser autenticado somente com o e-mail e senha cadastrados</t>
   </si>
   <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>Tela de Login
 (front-end)</t>
   </si>
@@ -106,7 +112,8 @@
     <t>Desejável</t>
   </si>
   <si>
-    <t>Banco de Dados</t>
+    <t>Banco de Dados
+(Nuvem e Backup)</t>
   </si>
   <si>
     <t>O software deverá registrar os dados em um banco de dados na nuvem contendo um backup local</t>
@@ -134,6 +141,9 @@
   </si>
   <si>
     <t>Os alertas serão exibidos em pop-ups assim que for constatado uma alteração extrema em um dos sensores instalados um determinado ambiente</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
   <si>
     <t>Tela Inical do Dashboard
@@ -174,6 +184,9 @@
     <t>Deve ser possível a visualização do gráfico com as cinco últimas médias incluindo a atual e média entre elas. Do lado direito irá conter as informações cadastradas para consulta rápida. Deverá também o redirecionamento para a consulta dos lotes naquele ambiente.</t>
   </si>
   <si>
+    <t>GG</t>
+  </si>
+  <si>
     <t>Telas dos Sensores
 (Back-end)</t>
   </si>
@@ -196,23 +209,41 @@
     <t>As informções devem ser retiradas e exibidas do banco de Dados</t>
   </si>
   <si>
+    <t>Protótipo de Tela
+(Site Institucional)</t>
+  </si>
+  <si>
+    <t>Os protótipos das Página Inicial deve ser simples, com informações resumidas e objetivas, contendo uma sessão para enviar os dados para solicitar um orçamento.</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>Protótipo de Tela
+(Dashboard)</t>
+  </si>
+  <si>
+    <t>As informações devem ser exibidas acompanhadas de funções visuais, como gráficos e a própia imagem do ambiente assim que o usuário acessar a plataforma</t>
+  </si>
+  <si>
+    <t>Banco de Dados
+(Criação)</t>
+  </si>
+  <si>
+    <t>O banco de dados deverá com as tabelas de Lote, ambiente, sensores, juntamente com as informações da Empresa e seus respectivos funcionários</t>
+  </si>
+  <si>
     <t xml:space="preserve">  Sprint Backlog: SPRINT 2 B - PROJETO DIWINE - Grupo 5</t>
   </si>
   <si>
     <t>PRIORIDADE</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,13 +262,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -494,29 +518,26 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -535,15 +556,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -552,13 +572,13 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -570,11 +590,11 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -584,7 +604,17 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -607,6 +637,36 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -627,111 +687,51 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
         </patternFill>
       </fill>
     </dxf>
@@ -796,11 +796,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right style="medium">
+        <right/>
+        <top/>
+        <bottom style="medium">
           <color rgb="FFC9C9C9"/>
-        </right>
-        <top/>
-        <bottom/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -829,7 +829,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right/>
+        <right style="medium">
+          <color rgb="FFC9C9C9"/>
+        </right>
         <top/>
         <bottom style="medium">
           <color rgb="FFC9C9C9"/>
@@ -853,6 +855,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
@@ -862,11 +865,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right style="medium">
+        <right/>
+        <top/>
+        <bottom style="medium">
           <color rgb="FFC9C9C9"/>
-        </right>
-        <top/>
-        <bottom/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -893,7 +896,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
           <color rgb="FFC9C9C9"/>
@@ -902,6 +905,8 @@
         <bottom style="medium">
           <color rgb="FFC9C9C9"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -928,106 +933,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color rgb="FFC9C9C9"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FFC9C9C9"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color rgb="FFC9C9C9"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
@@ -1039,109 +944,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color rgb="FFC9C9C9"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color rgb="FFC9C9C9"/>
-        </right>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FFC9C9C9"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color rgb="FFC9C9C9"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1184,41 +986,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFEDEDED"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFC9C9C9"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFC9C9C9"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="medium">
           <color rgb="FFA5A5A5"/>
@@ -1347,51 +1114,91 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1423,19 +1230,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{93BD3079-F089-44C3-8C40-5BEBC3CBFAD9}" name="Tabela4" displayName="Tabela4" ref="C3:I21" headerRowDxfId="32" dataDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30">
-  <autoFilter ref="C3:I21" xr:uid="{93BD3079-F089-44C3-8C40-5BEBC3CBFAD9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{93BD3079-F089-44C3-8C40-5BEBC3CBFAD9}" name="Tabela4" displayName="Tabela4" ref="C3:I27" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21">
+  <autoFilter ref="C3:I27" xr:uid="{93BD3079-F089-44C3-8C40-5BEBC3CBFAD9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:H13">
     <sortCondition descending="1" ref="H3:H13"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{36E880E4-916E-408F-9ADA-27042CECB835}" name="REQUISITO" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{D8DDA5BF-58B1-4AB4-88BF-E3A756B5B1E3}" name="DESCRIÇÃO" dataDxfId="25" totalsRowDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{30B7566E-7078-4652-8F6F-03EBB14A7BD3}" name="CLASSIFICAÇÃO" dataDxfId="23" totalsRowDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{9811019D-7C26-44C2-8FC5-702021479048}" name="FUNCIONALIDADE" dataDxfId="21" totalsRowDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{32479D40-A407-49AA-A8FF-0BE375C8B00D}" name="TAMANHO" dataDxfId="19" totalsRowDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{B0EB5ECB-B2AE-4132-A7E9-679B10665560}" name="TAM (#)" dataDxfId="17" totalsRowDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{7A9296CF-AC69-447A-B252-2B8D46350DCC}" name="SPRINT" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{36E880E4-916E-408F-9ADA-27042CECB835}" name="REQUISITO" totalsRowLabel="Total" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{D8DDA5BF-58B1-4AB4-88BF-E3A756B5B1E3}" name="DESCRIÇÃO" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{30B7566E-7078-4652-8F6F-03EBB14A7BD3}" name="CLASSIFICAÇÃO" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{9811019D-7C26-44C2-8FC5-702021479048}" name="FUNCIONALIDADE" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{32479D40-A407-49AA-A8FF-0BE375C8B00D}" name="TAMANHO" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{B0EB5ECB-B2AE-4132-A7E9-679B10665560}" name="TAM (#)" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{7A9296CF-AC69-447A-B252-2B8D46350DCC}" name="SPRINT" totalsRowFunction="count" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1741,44 +1548,44 @@
   <dimension ref="C3:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="84.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="86.140625" customWidth="1"/>
     <col min="5" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="15" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="13" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="15.75" thickBot="1">
-      <c r="C3" s="7" t="s">
+    <row r="3" spans="3:9">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+    <row r="4" spans="3:9" ht="50.1" customHeight="1">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1791,18 +1598,22 @@
       <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="10" t="s">
+      <c r="G4" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="50.1" customHeight="1">
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
@@ -1811,21 +1622,21 @@
         <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="2">
         <v>5</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="I5" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" ht="50.1" customHeight="1">
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>9</v>
@@ -1833,37 +1644,45 @@
       <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" ht="56.25" customHeight="1" thickBot="1">
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="4">
+        <v>8</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" ht="56.25" customHeight="1">
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" ht="50.1" customHeight="1">
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>9</v>
@@ -1871,56 +1690,68 @@
       <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="10" t="s">
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4">
+        <v>13</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" ht="50.1" customHeight="1">
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="H9" s="2">
+        <v>13</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="50.1" customHeight="1">
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="G10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="4">
+        <v>3</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" ht="50.1" customHeight="1">
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
@@ -1928,18 +1759,22 @@
       <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" ht="60" customHeight="1" thickBot="1">
+      <c r="G11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="2">
+        <v>13</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" ht="60" customHeight="1">
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>9</v>
@@ -1947,18 +1782,22 @@
       <c r="F12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" ht="56.25" customHeight="1" thickBot="1">
+      <c r="G12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="4">
+        <v>8</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" ht="56.25" customHeight="1">
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
@@ -1966,18 +1805,22 @@
       <c r="F13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" ht="58.5" customHeight="1" thickBot="1">
+      <c r="G13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2">
+        <v>8</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" ht="58.5" customHeight="1">
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>9</v>
@@ -1985,18 +1828,22 @@
       <c r="F14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="G14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="4">
+        <v>13</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" ht="50.1" customHeight="1">
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>
@@ -2004,18 +1851,22 @@
       <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="G15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="2">
+        <v>13</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" ht="50.1" customHeight="1">
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>9</v>
@@ -2023,18 +1874,22 @@
       <c r="F16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="G16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="4">
+        <v>21</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" ht="50.1" customHeight="1">
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>9</v>
@@ -2042,37 +1897,45 @@
       <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="G17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="2">
+        <v>21</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" ht="50.1" customHeight="1">
       <c r="C18" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
+      <c r="G18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="4">
+        <v>8</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" ht="50.1" customHeight="1">
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>9</v>
@@ -2080,97 +1943,183 @@
       <c r="F19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="3:9" ht="50.1" customHeight="1" thickBot="1">
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="12"/>
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2">
+        <v>8</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" ht="50.1" customHeight="1">
+      <c r="C20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="4">
+        <v>5</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" ht="50.1" customHeight="1">
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2">
+        <v>5</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="22" spans="3:9" ht="50.1" customHeight="1">
-      <c r="I22"/>
+      <c r="C22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="4">
+        <v>3</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="23" spans="3:9" ht="50.1" customHeight="1">
-      <c r="I23"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="3:9" ht="50.1" customHeight="1">
-      <c r="I24"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="3:9" ht="50.1" customHeight="1">
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="13"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="11"/>
     </row>
     <row r="26" spans="3:9" ht="50.1" customHeight="1">
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="3:9" ht="50.1" customHeight="1"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="3:9" ht="50.1" customHeight="1">
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="11"/>
+    </row>
     <row r="28" spans="3:9" ht="50.1" customHeight="1"/>
     <row r="29" spans="3:9" ht="50.1" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="H1:H12 I15:I17 H14:H1048576 I19">
-    <cfRule type="cellIs" dxfId="43" priority="20" operator="equal">
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="38" priority="16" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
+      <formula>"PP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="28" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
+      <formula>"M"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:I17 I19 I23 H1:H1048576">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="37" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="38" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="40" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G12 G14:G1048576">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
-      <formula>"GG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
-      <formula>"PP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
-      <formula>"G"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="14" operator="equal">
-      <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
-      <formula>"P"</formula>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2184,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06E1FE0-7E7C-41AC-A43D-6429ADC6CC4F}">
   <dimension ref="B1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2203,199 +2152,191 @@
     <row r="1" spans="2:9" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:9" ht="14.25" customHeight="1" thickBot="1"/>
     <row r="3" spans="2:9" ht="42" customHeight="1">
-      <c r="B3" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
+      <c r="B3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="2:9" ht="19.5" customHeight="1">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="29" t="s">
+      <c r="H4" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="50.1" customHeight="1" thickBot="1">
-      <c r="B5" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="20">
+      <c r="F5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="18">
         <v>5</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="18">
         <v>1</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="50.1" customHeight="1">
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B6" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="17" t="s">
+      <c r="G6" s="15"/>
+      <c r="H6" s="15">
+        <v>2</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="50.1" customHeight="1">
+      <c r="B7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="18">
+        <v>13</v>
+      </c>
+      <c r="H7" s="18">
+        <v>1</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="50.1" customHeight="1">
+      <c r="B8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17">
+      <c r="G8" s="20">
+        <v>8</v>
+      </c>
+      <c r="H8" s="20">
         <v>2</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B7" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="20">
-        <v>13</v>
-      </c>
-      <c r="H7" s="20">
-        <v>1</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B8" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="22">
-        <v>8</v>
-      </c>
-      <c r="H8" s="22">
-        <v>2</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>15</v>
+      <c r="I8" s="21" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="G5:G8 H4:H8">
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="G4 F4:F8">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+      <formula>"PP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"M"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H2 H4:H10 D11:D18 H19:H1048576">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H8 G5:G8">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
       <formula>5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F8 G4">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>"GG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"PP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"G"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H2 H4:H10 H19:H1048576 D11:D18">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Criação do gráfico de BurnDown
</commit_message>
<xml_diff>
--- a/Tecnologia da Informação/Backlog.xlsx
+++ b/Tecnologia da Informação/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/giulia_ayres_sptech_school/Documents/Giulia/Projeto-Diwine/Tecnologia da Informação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1330" documentId="8_{F8D6D5E0-FEAD-4D71-95E1-08BB12FF2741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A5B2921-2C99-4B22-B525-CB0128646360}"/>
+  <xr:revisionPtr revIDLastSave="1333" documentId="8_{F8D6D5E0-FEAD-4D71-95E1-08BB12FF2741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B578A587-A120-43E9-8269-20F31ADE87CC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9BAA43A6-2120-409E-B19A-63F3A8B8DC14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9BAA43A6-2120-409E-B19A-63F3A8B8DC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -714,15 +714,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -739,6 +730,15 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="G" xfId="2" xr:uid="{9E8260A5-C24A-4AC3-A086-B98A1C97C569}"/>
@@ -746,6 +746,526 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="113">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -808,11 +1328,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color theme="4" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFF7979"/>
         </patternFill>
       </fill>
     </dxf>
@@ -828,11 +1348,51 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="4" tint="-0.499984740745262"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF7979"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -843,6 +1403,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
         </patternFill>
       </fill>
     </dxf>
@@ -958,86 +1528,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF002060"/>
       </font>
       <fill>
@@ -1063,106 +1553,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1223,396 +1613,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2110,6 +2110,85 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>86925</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5DE4EF1-D86B-AD70-3E00-859A45B7C223}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="693963" y="381001"/>
+          <a:ext cx="9190105" cy="5143500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -2432,7 +2511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C378730-FC8F-4479-A9F9-487C359D13A9}">
   <dimension ref="C2:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -2471,10 +2550,10 @@
       <c r="I3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="35" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2500,10 +2579,10 @@
       <c r="I4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="40" t="s">
+      <c r="L4" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="40">
+      <c r="M4" s="37">
         <v>13</v>
       </c>
     </row>
@@ -2529,10 +2608,10 @@
       <c r="I5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="41" t="s">
+      <c r="L5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="38">
         <v>29</v>
       </c>
     </row>
@@ -2558,10 +2637,10 @@
       <c r="I6" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="L6" s="40" t="s">
+      <c r="L6" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="40">
+      <c r="M6" s="37">
         <v>31</v>
       </c>
     </row>
@@ -2587,10 +2666,10 @@
       <c r="I7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="41" t="s">
+      <c r="L7" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="M7" s="41">
+      <c r="M7" s="38">
         <f>SUM(H17,H19)</f>
         <v>29</v>
       </c>
@@ -2617,10 +2696,10 @@
       <c r="I8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="42" t="s">
+      <c r="L8" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="42">
+      <c r="M8" s="39">
         <f>SUM(M4:M7)</f>
         <v>102</v>
       </c>
@@ -2647,10 +2726,10 @@
       <c r="I9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="43" t="s">
+      <c r="L9" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="M9" s="43">
+      <c r="M9" s="40">
         <v>25.5</v>
       </c>
     </row>
@@ -2699,7 +2778,7 @@
       <c r="I11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="39"/>
+      <c r="L11" s="36"/>
     </row>
     <row r="12" spans="3:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
@@ -3046,7 +3125,7 @@
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:I17 I19 I23 H1:H25 H27:H1048576">
+  <conditionalFormatting sqref="H1:H25 I15:I17 I19 I23 H27:H1048576">
     <cfRule type="cellIs" dxfId="96" priority="40" operator="equal">
       <formula>21</formula>
     </cfRule>
@@ -3081,19 +3160,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="1" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="3" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="4" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3109,7 +3188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06E1FE0-7E7C-41AC-A43D-6429ADC6CC4F}">
   <dimension ref="A1:XFC3872"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -3130,16 +3209,16 @@
     <row r="1" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="43"/>
     </row>
     <row r="4" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="24" t="s">
@@ -3247,16 +3326,16 @@
     </row>
     <row r="8" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
     </row>
     <row r="10" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="24" t="s">
@@ -3390,16 +3469,16 @@
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="43"/>
     </row>
     <row r="17" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="24" t="s">
@@ -3501,16 +3580,16 @@
     </row>
     <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
     </row>
     <row r="23" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="24" t="s">
@@ -23849,288 +23928,288 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="F5:F7">
-    <cfRule type="cellIs" dxfId="86" priority="144" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="145" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="148" operator="equal">
+      <formula>"M"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="147" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="146" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="147" operator="equal">
-      <formula>"G"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="148" operator="equal">
-      <formula>"M"</formula>
+    <cfRule type="cellIs" dxfId="77" priority="144" operator="equal">
+      <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:F20">
-    <cfRule type="cellIs" dxfId="81" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="109" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="110" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="111" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="112" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="113" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:F26">
-    <cfRule type="cellIs" dxfId="76" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:G4">
-    <cfRule type="cellIs" dxfId="71" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="189" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="188" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="189" operator="equal">
-      <formula>"GG"</formula>
+    <cfRule type="cellIs" dxfId="64" priority="192" operator="equal">
+      <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="190" operator="equal">
-      <formula>"PP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="191" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="192" operator="equal">
-      <formula>"M"</formula>
+    <cfRule type="cellIs" dxfId="62" priority="190" operator="equal">
+      <formula>"PP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:G17">
-    <cfRule type="cellIs" dxfId="66" priority="154" operator="equal">
-      <formula>"P"</formula>
+    <cfRule type="cellIs" dxfId="61" priority="156" operator="equal">
+      <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="158" operator="equal">
+      <formula>"M"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="157" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="155" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="156" operator="equal">
-      <formula>"PP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="157" operator="equal">
-      <formula>"G"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="158" operator="equal">
-      <formula>"M"</formula>
+    <cfRule type="cellIs" dxfId="57" priority="154" operator="equal">
+      <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:G23">
-    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="72" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="73" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="74" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="75" operator="equal">
       <formula>"M"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="71" operator="equal">
+      <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G7">
-    <cfRule type="cellIs" dxfId="56" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="149" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="151" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="152" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="153" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10 F10:F14">
-    <cfRule type="cellIs" dxfId="52" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="167" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="164" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="165" operator="equal">
-      <formula>"GG"</formula>
+    <cfRule type="cellIs" dxfId="45" priority="168" operator="equal">
+      <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="166" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="167" operator="equal">
-      <formula>"G"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="168" operator="equal">
-      <formula>"M"</formula>
+    <cfRule type="cellIs" dxfId="43" priority="165" operator="equal">
+      <formula>"GG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G19">
-    <cfRule type="cellIs" dxfId="47" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="128" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="126" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="124" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="125" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="126" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="127" operator="equal">
       <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="128" operator="equal">
-      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24:G26">
-    <cfRule type="cellIs" dxfId="42" priority="16" operator="equal">
-      <formula>21</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="18" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="19" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
       <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+      <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:H7">
-    <cfRule type="cellIs" dxfId="37" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="95" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:H20">
-    <cfRule type="cellIs" dxfId="36" priority="114" operator="equal">
-      <formula>21</formula>
+    <cfRule type="cellIs" dxfId="31" priority="117" operator="equal">
+      <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="118" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="115" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="116" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="117" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="118" operator="equal">
-      <formula>5</formula>
+    <cfRule type="cellIs" dxfId="27" priority="114" operator="equal">
+      <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H2 H4:H8 H10:H14 D15 H17 H21 H23 H16401:H1048576">
-    <cfRule type="cellIs" dxfId="31" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="185" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="187" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4 I26">
-    <cfRule type="cellIs" dxfId="29" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="195" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H7">
-    <cfRule type="cellIs" dxfId="28" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="94" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="96" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="97" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="98" operator="equal">
       <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="96" operator="equal">
+      <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:H14 G11:G14">
-    <cfRule type="cellIs" dxfId="24" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="170" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="169" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="170" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="171" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="172" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="173" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:H14 H17 H4:H8 H23 H1:H2 D15 H21 H16401:H1048576">
-    <cfRule type="cellIs" dxfId="19" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="184" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="18" priority="159" operator="equal">
-      <formula>21</formula>
+    <cfRule type="cellIs" dxfId="13" priority="161" operator="equal">
+      <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="162" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="163" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="160" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="161" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="162" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="163" operator="equal">
-      <formula>5</formula>
+    <cfRule type="cellIs" dxfId="9" priority="159" operator="equal">
+      <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="13" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="80" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="77" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="76" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="77" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="78" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="79" operator="equal">
       <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="80" operator="equal">
-      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="cellIs" dxfId="8" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="194" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="196" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="197" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="198" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24142,13 +24221,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3392793-B919-45CF-9776-0F5E4234C01A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Criaçãodo gráfico de BurnDown
</commit_message>
<xml_diff>
--- a/Tecnologia da Informação/Backlog.xlsx
+++ b/Tecnologia da Informação/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/giulia_ayres_sptech_school/Documents/Giulia/Projeto-Diwine/Tecnologia da Informação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1333" documentId="8_{F8D6D5E0-FEAD-4D71-95E1-08BB12FF2741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B578A587-A120-43E9-8269-20F31ADE87CC}"/>
+  <xr:revisionPtr revIDLastSave="1367" documentId="8_{F8D6D5E0-FEAD-4D71-95E1-08BB12FF2741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86068E68-ED95-4A97-A84C-47F413357E57}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9BAA43A6-2120-409E-B19A-63F3A8B8DC14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{9BAA43A6-2120-409E-B19A-63F3A8B8DC14}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>A tela deve conter em formato de grade os Ambientes criados com seus respectivos nomes e ID sendo um deles para redirecionameto de criação de ambiente, contendo também um menu lateral com redirecionamento para os dados de umidade e temperatura, perfil do funcionário logado.</t>
   </si>
   <si>
-    <t>SP2</t>
-  </si>
-  <si>
     <t>Tela Inical do Dashboard
 (back-end)</t>
   </si>
@@ -272,6 +269,9 @@
   </si>
   <si>
     <t>Média</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sprint Backlog: SPRINT 2 D - PROJETO DIWINE - Grupo 5</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="113">
+  <dxfs count="128">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -773,296 +773,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1128,11 +838,41 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1153,76 +893,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7979"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF93B7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1328,11 +998,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="4" tint="-0.499984740745262"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF7979"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1348,6 +1018,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1358,11 +1068,71 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF002060"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1403,6 +1173,236 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1518,11 +1518,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1538,11 +1548,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="4" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1558,11 +1578,141 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="4" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF93B7FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2115,22 +2265,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>81642</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>86925</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>379492</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
+        <xdr:cNvPr id="4" name="Imagem 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5DE4EF1-D86B-AD70-3E00-859A45B7C223}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E19F5960-35F3-C74E-CD89-3116C0623EF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2139,49 +2289,25 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="693963" y="381001"/>
-          <a:ext cx="9190105" cy="5143500"/>
+          <a:off x="612321" y="204106"/>
+          <a:ext cx="10788957" cy="6068787"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF">
-            <a:shade val="85000"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln w="88900" cap="sq">
-          <a:solidFill>
-            <a:srgbClr val="FFFFFF"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="40000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="twoPt" dir="t">
-            <a:rot lat="0" lon="0" rev="7200000"/>
-          </a:lightRig>
-        </a:scene3d>
-        <a:sp3d>
-          <a:bevelT w="25400" h="19050"/>
-          <a:contourClr>
-            <a:srgbClr val="FFFFFF"/>
-          </a:contourClr>
-        </a:sp3d>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2194,19 +2320,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{93BD3079-F089-44C3-8C40-5BEBC3CBFAD9}" name="Tabela4" displayName="Tabela4" ref="C3:I27" headerRowDxfId="112" dataDxfId="110" headerRowBorderDxfId="111" tableBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{93BD3079-F089-44C3-8C40-5BEBC3CBFAD9}" name="Tabela4" displayName="Tabela4" ref="C3:I27" headerRowDxfId="127" dataDxfId="125" headerRowBorderDxfId="126" tableBorderDxfId="124">
   <autoFilter ref="C3:I27" xr:uid="{93BD3079-F089-44C3-8C40-5BEBC3CBFAD9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:H13">
     <sortCondition descending="1" ref="H3:H13"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{36E880E4-916E-408F-9ADA-27042CECB835}" name="REQUISITO" totalsRowLabel="Total" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{D8DDA5BF-58B1-4AB4-88BF-E3A756B5B1E3}" name="DESCRIÇÃO" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{30B7566E-7078-4652-8F6F-03EBB14A7BD3}" name="CLASSIFICAÇÃO" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{9811019D-7C26-44C2-8FC5-702021479048}" name="FUNCIONALIDADE" dataDxfId="105"/>
-    <tableColumn id="5" xr3:uid="{32479D40-A407-49AA-A8FF-0BE375C8B00D}" name="TAMANHO" dataDxfId="104"/>
-    <tableColumn id="6" xr3:uid="{B0EB5ECB-B2AE-4132-A7E9-679B10665560}" name="TAM (#)" dataDxfId="103"/>
-    <tableColumn id="11" xr3:uid="{7A9296CF-AC69-447A-B252-2B8D46350DCC}" name="SPRINT" totalsRowFunction="count" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{36E880E4-916E-408F-9ADA-27042CECB835}" name="REQUISITO" totalsRowLabel="Total" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{D8DDA5BF-58B1-4AB4-88BF-E3A756B5B1E3}" name="DESCRIÇÃO" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{30B7566E-7078-4652-8F6F-03EBB14A7BD3}" name="CLASSIFICAÇÃO" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{9811019D-7C26-44C2-8FC5-702021479048}" name="FUNCIONALIDADE" dataDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{32479D40-A407-49AA-A8FF-0BE375C8B00D}" name="TAMANHO" dataDxfId="119"/>
+    <tableColumn id="6" xr3:uid="{B0EB5ECB-B2AE-4132-A7E9-679B10665560}" name="TAM (#)" dataDxfId="118"/>
+    <tableColumn id="11" xr3:uid="{7A9296CF-AC69-447A-B252-2B8D46350DCC}" name="SPRINT" totalsRowFunction="count" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2511,8 +2637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C378730-FC8F-4479-A9F9-487C359D13A9}">
   <dimension ref="C2:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2551,10 +2677,10 @@
         <v>6</v>
       </c>
       <c r="L3" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="35" t="s">
         <v>68</v>
-      </c>
-      <c r="M3" s="35" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="3:13" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2577,10 +2703,10 @@
         <v>5</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M4" s="37">
         <v>13</v>
@@ -2635,10 +2761,10 @@
         <v>8</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M6" s="37">
         <v>31</v>
@@ -2667,11 +2793,10 @@
         <v>16</v>
       </c>
       <c r="L7" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M7" s="38">
-        <f>SUM(H17,H19)</f>
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="3:13" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2697,11 +2822,11 @@
         <v>12</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M8" s="39">
         <f>SUM(M4:M7)</f>
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="3:13" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2712,10 +2837,10 @@
         <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>11</v>
@@ -2727,10 +2852,10 @@
         <v>16</v>
       </c>
       <c r="L9" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M9" s="40">
-        <v>25.5</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="10" spans="3:13" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2800,15 +2925,15 @@
         <v>5</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="3:13" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
@@ -2828,10 +2953,10 @@
     </row>
     <row r="14" spans="3:13" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>9</v>
@@ -2846,15 +2971,15 @@
         <v>5</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="3:13" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>
@@ -2874,10 +2999,10 @@
     </row>
     <row r="16" spans="3:13" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>9</v>
@@ -2886,21 +3011,21 @@
         <v>10</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16" s="4">
         <v>21</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="3:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>9</v>
@@ -2909,7 +3034,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H17" s="2">
         <v>21</v>
@@ -2920,10 +3045,10 @@
     </row>
     <row r="18" spans="3:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>22</v>
@@ -2938,15 +3063,15 @@
         <v>8</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="3:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>9</v>
@@ -2966,10 +3091,10 @@
     </row>
     <row r="20" spans="3:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>22</v>
@@ -2984,15 +3109,15 @@
         <v>5</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>9</v>
@@ -3007,15 +3132,15 @@
         <v>5</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="3:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>9</v>
@@ -3030,15 +3155,15 @@
         <v>3</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="3:9" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>30</v>
@@ -3053,12 +3178,12 @@
         <v>13</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="3:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="33"/>
       <c r="E24" s="33" t="s">
@@ -3074,7 +3199,7 @@
         <v>5</v>
       </c>
       <c r="I24" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="3:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3109,70 +3234,70 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="101" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="21" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="31" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="32" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="33" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="34" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H25 I15:I17 I19 I23 H27:H1048576">
-    <cfRule type="cellIs" dxfId="96" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="40" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="42" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="43" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="44" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="45" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="cellIs" dxfId="91" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="6" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="8" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="9" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="10" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="cellIs" dxfId="86" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="1" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="3" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="4" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3188,8 +3313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06E1FE0-7E7C-41AC-A43D-6429ADC6CC4F}">
   <dimension ref="A1:XFC3872"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3198,7 +3323,8 @@
     <col min="2" max="2" width="24.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="84.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="5" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="5" customWidth="1"/>
     <col min="7" max="8" width="15.7109375" style="5" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" style="5" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="5"/>
@@ -3210,7 +3336,7 @@
     <row r="2" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
@@ -3240,7 +3366,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="24" t="s">
         <v>6</v>
@@ -3248,10 +3374,10 @@
     </row>
     <row r="5" spans="2:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>52</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>22</v>
@@ -3269,15 +3395,15 @@
         <v>2</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
@@ -3295,15 +3421,15 @@
         <v>2</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>55</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>56</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>9</v>
@@ -3321,13 +3447,13 @@
         <v>2</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
@@ -3357,7 +3483,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" s="24" t="s">
         <v>6</v>
@@ -3470,7 +3596,7 @@
     <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="42"/>
@@ -3500,7 +3626,7 @@
         <v>5</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>6</v>
@@ -3525,9 +3651,11 @@
       <c r="G18" s="26">
         <v>5</v>
       </c>
-      <c r="H18" s="27"/>
+      <c r="H18" s="18">
+        <v>1</v>
+      </c>
       <c r="I18" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3549,17 +3677,19 @@
       <c r="G19" s="26">
         <v>8</v>
       </c>
-      <c r="H19" s="30"/>
+      <c r="H19" s="18">
+        <v>1</v>
+      </c>
       <c r="I19" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>30</v>
@@ -3573,15 +3703,17 @@
       <c r="G20" s="18">
         <v>8</v>
       </c>
-      <c r="H20" s="19"/>
+      <c r="H20" s="20">
+        <v>2</v>
+      </c>
       <c r="I20" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="41" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>
@@ -3611,7 +3743,7 @@
         <v>5</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I23" s="24" t="s">
         <v>6</v>
@@ -3638,15 +3770,15 @@
       </c>
       <c r="H24" s="30"/>
       <c r="I24" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:9" customFormat="1" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="33" t="s">
         <v>39</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>40</v>
       </c>
       <c r="D25" s="33" t="s">
         <v>9</v>
@@ -3662,15 +3794,15 @@
       </c>
       <c r="H25" s="27"/>
       <c r="I25" s="34" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:9" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
@@ -3679,14 +3811,14 @@
         <v>10</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G26" s="4">
         <v>21</v>
       </c>
       <c r="H26" s="30"/>
-      <c r="I26" s="9" t="s">
-        <v>36</v>
+      <c r="I26" s="21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="2:9" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
@@ -23928,288 +24060,339 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="F5:F7">
-    <cfRule type="cellIs" dxfId="81" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="159" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="160" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="148" operator="equal">
-      <formula>"M"</formula>
+    <cfRule type="cellIs" dxfId="94" priority="161" operator="equal">
+      <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="162" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="146" operator="equal">
-      <formula>"PP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="144" operator="equal">
-      <formula>"P"</formula>
+    <cfRule type="cellIs" dxfId="92" priority="163" operator="equal">
+      <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:F20">
-    <cfRule type="cellIs" dxfId="76" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="124" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="125" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="126" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="127" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="128" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:F26">
-    <cfRule type="cellIs" dxfId="71" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="16" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="17" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="18" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="19" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
       <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:G4">
-    <cfRule type="cellIs" dxfId="66" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="203" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="204" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="188" operator="equal">
-      <formula>"P"</formula>
+    <cfRule type="cellIs" dxfId="79" priority="205" operator="equal">
+      <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="192" operator="equal">
-      <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="206" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="190" operator="equal">
-      <formula>"PP"</formula>
+    <cfRule type="cellIs" dxfId="77" priority="207" operator="equal">
+      <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:G17">
-    <cfRule type="cellIs" dxfId="61" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="169" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="170" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="171" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="158" operator="equal">
-      <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="172" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="155" operator="equal">
-      <formula>"GG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="154" operator="equal">
-      <formula>"P"</formula>
+    <cfRule type="cellIs" dxfId="72" priority="173" operator="equal">
+      <formula>"M"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:G23">
-    <cfRule type="cellIs" dxfId="56" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="86" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="87" operator="equal">
       <formula>"GG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="88" operator="equal">
       <formula>"PP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="89" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="90" operator="equal">
       <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="71" operator="equal">
-      <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G7">
-    <cfRule type="cellIs" dxfId="51" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="164" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="166" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="167" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="168" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10 F10:F14">
-    <cfRule type="cellIs" dxfId="47" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="179" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="180" operator="equal">
+      <formula>"GG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="181" operator="equal">
+      <formula>"PP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="182" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="164" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="183" operator="equal">
       <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="166" operator="equal">
-      <formula>"PP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="165" operator="equal">
-      <formula>"GG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G19">
-    <cfRule type="cellIs" dxfId="42" priority="128" operator="equal">
-      <formula>5</formula>
+    <cfRule type="cellIs" dxfId="57" priority="139" operator="equal">
+      <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="140" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="141" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="124" operator="equal">
-      <formula>21</formula>
+    <cfRule type="cellIs" dxfId="54" priority="142" operator="equal">
+      <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="125" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="127" operator="equal">
-      <formula>8</formula>
+    <cfRule type="cellIs" dxfId="53" priority="143" operator="equal">
+      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24:G26">
-    <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="31" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="32" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="33" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="34" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="35" operator="equal">
       <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
-      <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:H7">
-    <cfRule type="cellIs" dxfId="32" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="110" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:H20">
-    <cfRule type="cellIs" dxfId="31" priority="117" operator="equal">
+  <conditionalFormatting sqref="G20">
+    <cfRule type="cellIs" dxfId="46" priority="129" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="130" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="131" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="132" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="133" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="115" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="116" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="114" operator="equal">
-      <formula>21</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H2 H4:H8 H10:H14 D15 H17 H21 H23 H16401:H1048576">
-    <cfRule type="cellIs" dxfId="26" priority="185" operator="equal">
+  <conditionalFormatting sqref="H1:H2 H4:H8 H10:H14 D15 H23 H16401:H1048576 H17:H21">
+    <cfRule type="cellIs" dxfId="41" priority="200" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="202" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4 I26">
-    <cfRule type="cellIs" dxfId="24" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="210" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H7">
-    <cfRule type="cellIs" dxfId="23" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="109" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="111" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="112" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="113" operator="equal">
       <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="96" operator="equal">
-      <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:H14 G11:G14">
-    <cfRule type="cellIs" dxfId="19" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="184" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="185" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="169" operator="equal">
-      <formula>21</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="186" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="187" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="188" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10:H14 H17 H4:H8 H23 H1:H2 D15 H21 H16401:H1048576">
-    <cfRule type="cellIs" dxfId="14" priority="184" operator="equal">
+  <conditionalFormatting sqref="H10:H14 H4:H8 H23 H1:H2 D15 H16401:H1048576 H17:H21">
+    <cfRule type="cellIs" dxfId="29" priority="199" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="13" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="174" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="175" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="176" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="177" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="178" operator="equal">
       <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="160" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="159" operator="equal">
-      <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="8" priority="80" operator="equal">
-      <formula>5</formula>
+    <cfRule type="cellIs" dxfId="23" priority="91" operator="equal">
+      <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="92" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="76" operator="equal">
-      <formula>21</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="93" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="94" operator="equal">
       <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="95" operator="equal">
+      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="cellIs" dxfId="3" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="209" operator="equal">
       <formula>21</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="211" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="212" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="213" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24221,8 +24404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3392793-B919-45CF-9776-0F5E4234C01A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X29" sqref="X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>